<commit_message>
Updated GOMS excel to contain all of the functions
added all functions Tobi has added to our application
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{091FC835-C27B-B440-AADF-EABBC38C892C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82435E97-6010-AF46-A8CC-AA8277DA142F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
@@ -35,11 +35,97 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Local IDE ( PYTHON ) in minutes</t>
+  </si>
+  <si>
+    <t>Data Polish</t>
+  </si>
+  <si>
+    <t>Normalization</t>
+  </si>
+  <si>
+    <t>Fill Missing Values</t>
+  </si>
+  <si>
+    <t>Outlier Removal</t>
+  </si>
+  <si>
+    <t>Numeric to Category</t>
+  </si>
+  <si>
+    <t>Principal Component Analysis</t>
+  </si>
+  <si>
+    <t>Change Column Type</t>
+  </si>
+  <si>
+    <t>Rename Column</t>
+  </si>
+  <si>
+    <t>Special Character Removal</t>
+  </si>
+  <si>
+    <t>Trim Whitespace</t>
+  </si>
+  <si>
+    <t>Replace Substrings</t>
+  </si>
+  <si>
+    <t>Text Case</t>
+  </si>
+  <si>
+    <t>Remove Stopwords</t>
+  </si>
+  <si>
+    <t>Collapse Rare Categories</t>
+  </si>
+  <si>
+    <t>Tokenization</t>
+  </si>
+  <si>
+    <t>Regex</t>
+  </si>
+  <si>
+    <t>Datetime Components</t>
+  </si>
+  <si>
+    <t>Remove Columns</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>TOTAL in hours</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -66,8 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +470,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCED56-B1F8-4349-9CA5-CFF48A33C9D8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added times taken for overall task in the GOMS excel
Added times taken for overall task in the GOMS excel
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82435E97-6010-AF46-A8CC-AA8277DA142F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBCC934-6947-8A4C-9381-798A8C0D36E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
@@ -497,133 +497,173 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>22</v>
+      </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>13</v>
+      </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>23</v>
+      </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>11</v>
+      </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>12</v>
+      </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>11</v>
+      </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>11</v>
+      </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>8</v>
+      </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1">
+        <f>SUM(B2:B18)</f>
+        <v>206</v>
+      </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1">
+        <f>B19/60</f>
+        <v>3.4333333333333331</v>
+      </c>
       <c r="C20" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Normalisation Results for Python IDE
added the time and code for GOMS for Python results
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBCC934-6947-8A4C-9381-798A8C0D36E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00449B1-2EF1-404C-AA5F-C01245418EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparison" sheetId="1" r:id="rId1"/>
+    <sheet name="Normalisation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Task</t>
   </si>
@@ -102,13 +103,61 @@
   </si>
   <si>
     <t>TOTAL in hours</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Upload CSV</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>df = pd.read_csv('file.csv')</t>
+  </si>
+  <si>
+    <t>Visualize Data</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>df.describe()</t>
+  </si>
+  <si>
+    <t>Apply Normalization</t>
+  </si>
+  <si>
+    <t>from sklearn.preprocessing import MinMaxScaler &lt;br&gt; scaler = MinMaxScaler() &lt;br&gt; df_scaled = pd.DataFrame(scaler.fit_transform(df), columns=df.columns)</t>
+  </si>
+  <si>
+    <t>Verify Normalization</t>
+  </si>
+  <si>
+    <t>2 min</t>
+  </si>
+  <si>
+    <t>df_scaled.describe()</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>22 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,6 +175,21 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -152,10 +216,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,4 +735,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE17A0E3-F5EC-554A-9735-BFFAD7E9361A}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done the same with Missing Values
added time taken and code for missing values in GOMS
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00449B1-2EF1-404C-AA5F-C01245418EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADF2DCB-1A57-2740-9036-B2AE544A384B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" activeTab="2" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Normalisation" sheetId="2" r:id="rId2"/>
+    <sheet name="Missing Values" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -151,13 +152,40 @@
   </si>
   <si>
     <t>22 min</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Check Missing Values</t>
+  </si>
+  <si>
+    <t>1 min</t>
+  </si>
+  <si>
+    <t>df.isnull().sum()</t>
+  </si>
+  <si>
+    <t>Choose Strategy</t>
+  </si>
+  <si>
+    <t>Decide on filling with mean, median, or mode</t>
+  </si>
+  <si>
+    <t>df.fillna(df.mean(), inplace=True)</t>
+  </si>
+  <si>
+    <t>Verify</t>
+  </si>
+  <si>
+    <t>13 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,6 +223,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,12 +259,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCED56-B1F8-4349-9CA5-CFF48A33C9D8}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
@@ -813,4 +858,94 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C172AB-F034-AC4C-971B-243D9D7B901D}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Outlier Removal Sheet
Goms outlier removal addition
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADF2DCB-1A57-2740-9036-B2AE544A384B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2163AD8-CEFB-8B43-8CEF-31ECC46504E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" activeTab="2" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" activeTab="3" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Normalisation" sheetId="2" r:id="rId2"/>
     <sheet name="Missing Values" sheetId="3" r:id="rId3"/>
+    <sheet name="Outlier Removal" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -179,13 +180,40 @@
   </si>
   <si>
     <t>13 min</t>
+  </si>
+  <si>
+    <t>Statistical Summary</t>
+  </si>
+  <si>
+    <t>df.describe() to identify outliers</t>
+  </si>
+  <si>
+    <t>Visualize Outliers</t>
+  </si>
+  <si>
+    <t>Use sns.boxplot(data=df)</t>
+  </si>
+  <si>
+    <t>Remove Outliers</t>
+  </si>
+  <si>
+    <t>Use IQR or Z-score method to filter out outliers</t>
+  </si>
+  <si>
+    <t>Verify Changes</t>
+  </si>
+  <si>
+    <t>Replot with sns.boxplot(data=df)</t>
+  </si>
+  <si>
+    <t>23 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,6 +266,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -259,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -267,6 +302,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,6 +900,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C172AB-F034-AC4C-971B-243D9D7B901D}">
   <dimension ref="A1:C7"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6030CA5-24BA-8741-A5E3-0CBEB6E20D49}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C7"/>
     </sheetView>
@@ -878,7 +1004,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -894,46 +1020,46 @@
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -941,9 +1067,9 @@
         <v>36</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="C7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Numeric to Categorical
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2163AD8-CEFB-8B43-8CEF-31ECC46504E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C1A6D2-DFC5-D540-9A9B-711197D35B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" activeTab="3" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" activeTab="4" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Normalisation" sheetId="2" r:id="rId2"/>
     <sheet name="Missing Values" sheetId="3" r:id="rId3"/>
     <sheet name="Outlier Removal" sheetId="4" r:id="rId4"/>
+    <sheet name="Numeric To Categorical" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>Task</t>
   </si>
@@ -207,6 +208,21 @@
   </si>
   <si>
     <t>23 min</t>
+  </si>
+  <si>
+    <t>Identify Numerics</t>
+  </si>
+  <si>
+    <t>df.select_dtypes(include=['int', 'float'])</t>
+  </si>
+  <si>
+    <t>Convert to Category</t>
+  </si>
+  <si>
+    <t>df['column'] = df['column'].astype('category')</t>
+  </si>
+  <si>
+    <t>df.info() to check new dtypes</t>
   </si>
 </sst>
 </file>
@@ -990,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6030CA5-24BA-8741-A5E3-0CBEB6E20D49}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
@@ -1074,4 +1090,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE8F680-674B-C845-897A-B307A627C944}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Rename Column Results
Added Rename Column Results into the GOMS excel from python IDE
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F573B9D-B98B-E146-B370-B41FF6A7FDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51A699C-D6B9-6C40-916C-4970A1FDAB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" activeTab="6" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" activeTab="7" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Numeric To Categorical" sheetId="5" r:id="rId5"/>
     <sheet name="Principal Component Analysis" sheetId="6" r:id="rId6"/>
     <sheet name="Change Column Type" sheetId="7" r:id="rId7"/>
+    <sheet name="Rename Column" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="77">
   <si>
     <t>Task</t>
   </si>
@@ -264,6 +265,15 @@
   </si>
   <si>
     <t>df.dtypes to confirm the change</t>
+  </si>
+  <si>
+    <t>df.rename(columns={'old_name': 'new_name'}, inplace=True)</t>
+  </si>
+  <si>
+    <t>df.head() to check new column names</t>
+  </si>
+  <si>
+    <t>7 min</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87741834-764D-8442-88E6-1252B0C99BC2}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -1365,4 +1375,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC10668-04B2-D949-B9DB-65DF0C8FBDE5}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Special Character Removal
Added Special Character Removal into GOMS EXCEL
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51A699C-D6B9-6C40-916C-4970A1FDAB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9404B8A4-B4EB-2B4A-B345-82477999C568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" activeTab="7" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="1" activeTab="8" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Principal Component Analysis" sheetId="6" r:id="rId6"/>
     <sheet name="Change Column Type" sheetId="7" r:id="rId7"/>
     <sheet name="Rename Column" sheetId="8" r:id="rId8"/>
+    <sheet name="Special Character Removal" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="82">
   <si>
     <t>Task</t>
   </si>
@@ -274,6 +275,21 @@
   </si>
   <si>
     <t>7 min</t>
+  </si>
+  <si>
+    <t>Identify Characters</t>
+  </si>
+  <si>
+    <t>Visual inspection with df.head()</t>
+  </si>
+  <si>
+    <t>Remove Characters</t>
+  </si>
+  <si>
+    <t>df.replace({r'[^\x00-\x7F]+':''}, regex=True, inplace=True)</t>
+  </si>
+  <si>
+    <t>df.head() to check cleaned data</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC10668-04B2-D949-B9DB-65DF0C8FBDE5}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -1442,4 +1458,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8945ED-BAF2-C34A-80C4-D30B68C8DA2C}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added Trim Whitespace results into GOMS
As description from python IDE
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9404B8A4-B4EB-2B4A-B345-82477999C568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC497B22-705F-C04A-843B-0582A0628D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="1" activeTab="8" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="3" activeTab="9" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Change Column Type" sheetId="7" r:id="rId7"/>
     <sheet name="Rename Column" sheetId="8" r:id="rId8"/>
     <sheet name="Special Character Removal" sheetId="9" r:id="rId9"/>
+    <sheet name="Trim Whitespace" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="85">
   <si>
     <t>Task</t>
   </si>
@@ -290,6 +291,15 @@
   </si>
   <si>
     <t>df.head() to check cleaned data</t>
+  </si>
+  <si>
+    <t>df = df.applymap(lambda x: x.strip() if isinstance(x, str) else x)</t>
+  </si>
+  <si>
+    <t>df.head() to check trimmed strings</t>
+  </si>
+  <si>
+    <t>8 min</t>
   </si>
 </sst>
 </file>
@@ -901,6 +911,73 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6062ED13-C528-F146-AE70-5ACC98E5FD07}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE17A0E3-F5EC-554A-9735-BFFAD7E9361A}">
   <dimension ref="A1:C6"/>
@@ -1464,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8945ED-BAF2-C34A-80C4-D30B68C8DA2C}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Replace Substrings to GOMS excel
python IDE
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC497B22-705F-C04A-843B-0582A0628D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3808CFE9-7ED9-404F-BCAA-538B2C2116A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="3" activeTab="9" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="10" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Rename Column" sheetId="8" r:id="rId8"/>
     <sheet name="Special Character Removal" sheetId="9" r:id="rId9"/>
     <sheet name="Trim Whitespace" sheetId="10" r:id="rId10"/>
+    <sheet name="Replace Substrings" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="90">
   <si>
     <t>Task</t>
   </si>
@@ -300,6 +301,21 @@
   </si>
   <si>
     <t>8 min</t>
+  </si>
+  <si>
+    <t>Identify Substrings</t>
+  </si>
+  <si>
+    <t>Use df['column'].unique() to find unique values</t>
+  </si>
+  <si>
+    <t>df['column'].str.replace('old_substring', 'new_substring', regex=True)</t>
+  </si>
+  <si>
+    <t>df['column'].unique() to check replacements</t>
+  </si>
+  <si>
+    <t>11 min</t>
   </si>
 </sst>
 </file>
@@ -915,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6062ED13-C528-F146-AE70-5ACC98E5FD07}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -971,6 +987,84 @@
       </c>
       <c r="B5" s="3" t="s">
         <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20D2886-70F8-A640-969D-1FFF78906280}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Text Case into GOMS
added PYTHON IDE results
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3808CFE9-7ED9-404F-BCAA-538B2C2116A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C6DE28-C9CA-BE4C-8705-655780035778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="10" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="11" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Special Character Removal" sheetId="9" r:id="rId9"/>
     <sheet name="Trim Whitespace" sheetId="10" r:id="rId10"/>
     <sheet name="Replace Substrings" sheetId="11" r:id="rId11"/>
+    <sheet name="Text Case" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
   <si>
     <t>Task</t>
   </si>
@@ -316,6 +317,21 @@
   </si>
   <si>
     <t>11 min</t>
+  </si>
+  <si>
+    <t>Identify Text Columns</t>
+  </si>
+  <si>
+    <t>Find string columns with df.select_dtypes(include=[object])</t>
+  </si>
+  <si>
+    <t>Convert Case</t>
+  </si>
+  <si>
+    <t>df['text_column'] = df['text_column'].str.lower() or .str.upper()</t>
+  </si>
+  <si>
+    <t>df['text_column'].head() to confirm the case conversion</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20D2886-70F8-A640-969D-1FFF78906280}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -1065,6 +1081,84 @@
       </c>
       <c r="B6" s="3" t="s">
         <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B17B441-DAD5-B14A-B665-039BC5DFC85A}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Tokenization and Collapse Rare Category
Added Tokenization and collapse rare category python IDE
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C6DE28-C9CA-BE4C-8705-655780035778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2499A5C-E15B-D641-B21C-B9C2911255B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="11" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="7" activeTab="13" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,9 @@
     <sheet name="Trim Whitespace" sheetId="10" r:id="rId10"/>
     <sheet name="Replace Substrings" sheetId="11" r:id="rId11"/>
     <sheet name="Text Case" sheetId="12" r:id="rId12"/>
+    <sheet name="Remove Stopwords" sheetId="13" r:id="rId13"/>
+    <sheet name="Collapse Rare Categories" sheetId="14" r:id="rId14"/>
+    <sheet name="Tokenization" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="112">
   <si>
     <t>Task</t>
   </si>
@@ -332,6 +335,57 @@
   </si>
   <si>
     <t>df['text_column'].head() to confirm the case conversion</t>
+  </si>
+  <si>
+    <t>Load Stopwords</t>
+  </si>
+  <si>
+    <t>from nltk.corpus import stopwords</t>
+  </si>
+  <si>
+    <t>Loop over text column to filter out stopwords</t>
+  </si>
+  <si>
+    <t>Print some text samples to check</t>
+  </si>
+  <si>
+    <t>12 min</t>
+  </si>
+  <si>
+    <t>Value Counts</t>
+  </si>
+  <si>
+    <t>counts = df['category_column'].value_counts()</t>
+  </si>
+  <si>
+    <t>Determine Threshold</t>
+  </si>
+  <si>
+    <t>Decide on a minimum count for categories to be kept</t>
+  </si>
+  <si>
+    <t>Collapse Categories</t>
+  </si>
+  <si>
+    <t>df['category_column'] = df['category_column'].apply(lambda x: 'Other' if counts[x] &lt; threshold else x)</t>
+  </si>
+  <si>
+    <t>df['category_column'].value_counts()</t>
+  </si>
+  <si>
+    <t>Load Tokenizer</t>
+  </si>
+  <si>
+    <t>from nltk.tokenize import word_tokenize</t>
+  </si>
+  <si>
+    <t>Tokenize Text</t>
+  </si>
+  <si>
+    <t>df['text_column'].apply(word_tokenize)</t>
+  </si>
+  <si>
+    <t>df['text_column'].head()</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1146,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B17B441-DAD5-B14A-B665-039BC5DFC85A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18058F80-552A-2B46-9A61-17D28D671D7E}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
@@ -1122,24 +1254,24 @@
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1150,7 +1282,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1158,7 +1290,174 @@
         <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2990E6A3-2F89-4543-9085-4F79AE6CF6C1}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B15306A-7E9E-EF49-BEA7-BC4B3796CCEF}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Regex (Regular Expressions) into GOMS
added REGEX into GOMS
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2499A5C-E15B-D641-B21C-B9C2911255B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF7CEEC-B763-1744-AF07-CBA80DDA5B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="7" activeTab="13" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="9" activeTab="15" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Remove Stopwords" sheetId="13" r:id="rId13"/>
     <sheet name="Collapse Rare Categories" sheetId="14" r:id="rId14"/>
     <sheet name="Tokenization" sheetId="15" r:id="rId15"/>
+    <sheet name="Regex (Regular Expressions)" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="116">
   <si>
     <t>Task</t>
   </si>
@@ -386,6 +387,18 @@
   </si>
   <si>
     <t>df['text_column'].head()</t>
+  </si>
+  <si>
+    <t>Define Regex Pattern</t>
+  </si>
+  <si>
+    <t>pattern = r'some_regex_pattern'</t>
+  </si>
+  <si>
+    <t>Apply Regex</t>
+  </si>
+  <si>
+    <t>df['text_column'].str.findall(pattern)</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2990E6A3-2F89-4543-9085-4F79AE6CF6C1}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
@@ -1465,6 +1478,84 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDFEC69-75A2-0441-AC67-AB453D872A52}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE17A0E3-F5EC-554A-9735-BFFAD7E9361A}">
   <dimension ref="A1:C6"/>

</xml_diff>

<commit_message>
added Datetime Components to GOMS
Python results
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF7CEEC-B763-1744-AF07-CBA80DDA5B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A2F4A4-004C-E54F-9522-FC5F9DCB96DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" firstSheet="9" activeTab="15" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="9" activeTab="16" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="Collapse Rare Categories" sheetId="14" r:id="rId14"/>
     <sheet name="Tokenization" sheetId="15" r:id="rId15"/>
     <sheet name="Regex (Regular Expressions)" sheetId="16" r:id="rId16"/>
+    <sheet name="Datetime Components" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="121">
   <si>
     <t>Task</t>
   </si>
@@ -399,6 +400,21 @@
   </si>
   <si>
     <t>df['text_column'].str.findall(pattern)</t>
+  </si>
+  <si>
+    <t>Convert to Datetime</t>
+  </si>
+  <si>
+    <t>df['datetime_column'] = pd.to_datetime(df['datetime_column'])</t>
+  </si>
+  <si>
+    <t>Extract Components</t>
+  </si>
+  <si>
+    <t>df['year'] = df['datetime_column'].dt.year etc. for month, day, etc.</t>
+  </si>
+  <si>
+    <t>df[['year', 'month', 'day']].head()</t>
   </si>
 </sst>
 </file>
@@ -1482,6 +1498,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDFEC69-75A2-0441-AC67-AB453D872A52}">
   <dimension ref="A1:C6"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6779DF32-F3C5-8D4E-BC6D-C6BF3912FD45}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C6"/>
     </sheetView>
@@ -1512,24 +1606,24 @@
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1540,7 +1634,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added Remove Columns to GOMS
Added Remove Columns python IDE results
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/PythonVSData-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A2F4A4-004C-E54F-9522-FC5F9DCB96DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846B3D8D-42EF-5B45-B471-2866B8544EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="9" activeTab="16" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1180" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="10" activeTab="17" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Tokenization" sheetId="15" r:id="rId15"/>
     <sheet name="Regex (Regular Expressions)" sheetId="16" r:id="rId16"/>
     <sheet name="Datetime Components" sheetId="18" r:id="rId17"/>
+    <sheet name="Remove Columns" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="126">
   <si>
     <t>Task</t>
   </si>
@@ -415,6 +416,21 @@
   </si>
   <si>
     <t>df[['year', 'month', 'day']].head()</t>
+  </si>
+  <si>
+    <t>Identify Columns</t>
+  </si>
+  <si>
+    <t>df.columns to list all columns</t>
+  </si>
+  <si>
+    <t>Drop Columns</t>
+  </si>
+  <si>
+    <t>df.drop(['column1', 'column2'], axis=1, inplace=True)</t>
+  </si>
+  <si>
+    <t>df.head() to ensure columns are dropped</t>
   </si>
 </sst>
 </file>
@@ -1576,7 +1592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6779DF32-F3C5-8D4E-BC6D-C6BF3912FD45}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
@@ -1643,6 +1659,84 @@
       </c>
       <c r="B6" s="3" t="s">
         <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6836C7B9-0B85-3A4B-822E-23EEAE7381E3}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>